<commit_message>
updated teaching survey sheets
</commit_message>
<xml_diff>
--- a/sa/Fall24_Teaching_Hours.xlsx
+++ b/sa/Fall24_Teaching_Hours.xlsx
@@ -37,7 +37,7 @@
     <t>(pre-semester)</t>
   </si>
   <si>
-    <t>Course</t>
+    <t>Course(s) and number(s) of sections</t>
   </si>
   <si>
     <t>Your name</t>
@@ -93,7 +93,7 @@
     <t>Coordinator (if any)</t>
   </si>
   <si>
-    <t>Would you be willing to share course materials with the UCWU Math Organizing Committee to support future instructors/TAs/FAs?</t>
+    <t>Would you be willing to share course materials with the Math Organizing Committee to support future instructors/TAs/FAs?</t>
   </si>
   <si>
     <t>9/16 - 9/22</t>
@@ -170,6 +170,24 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
+      <t>—If you are teaching more than one course, you may use one sheet for each course or combine your hours in a single sheet</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
       <t xml:space="preserve">—To help keep track of time, we suggest using an app like </t>
     </r>
     <r>
@@ -183,6 +201,7 @@
     </r>
     <r>
       <rPr>
+        <b val="1"/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -205,7 +224,7 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t xml:space="preserve">(2) Please enter other course information in column E and your personal information in column G.
+      <t xml:space="preserve">(2) Please enter other course information in column E and your personal information in column G.  If you are recording multiple courses on this sheet, please indicate for each course as appropriate.
 </t>
     </r>
     <r>
@@ -223,7 +242,7 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t xml:space="preserve">(3) At the end of the term, the UCWU Math Organizing Committee will reach out with instructions to submit this spreadsheet.
+      <t xml:space="preserve">(3) At the end of the term, the Math Organizing Committee will reach out with instructions to submit this spreadsheet.
 </t>
     </r>
     <r>

</xml_diff>